<commit_message>
changed function GetIdList as GetIDList
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel_Ini/Item.xlsx
+++ b/_Out/NFDataCfg/Excel_Ini/Item.xlsx
@@ -854,6 +854,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -861,7 +868,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -885,6 +892,28 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -892,15 +921,31 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -914,54 +959,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -975,16 +975,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1036,19 +1036,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1060,13 +1084,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1078,37 +1156,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1132,79 +1192,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1283,6 +1283,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1303,15 +1318,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1328,30 +1334,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1362,6 +1344,24 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1385,7 +1385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1403,130 +1403,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1960,7 +1960,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E$1:E$1048576"/>
+      <selection pane="bottomRight" activeCell="A138" sqref="A138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>

</xml_diff>

<commit_message>
new gift for new player
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel_Ini/Item.xlsx
+++ b/_Out/NFDataCfg/Excel_Ini/Item.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286">
   <si>
     <t>Id</t>
   </si>
@@ -447,6 +447,9 @@
     <t>Desc_NoobPack</t>
   </si>
   <si>
+    <t>Item_HOLY_WATER_1,11;Item_HOLY_WATER_2,22;Item_HOLY_WATER_3,33;Item_HOLY_WATER_4,44;Item_HOLY_WATER_5,55;Item_MP1,11;Item_MP2,22;Item_MP3,33;Item_MP4,44;Item_MP5,55;Item_GEM_ATK_1,11;Item_GEM_ATK_2,22;Item_GEM_ATK_3,33;Item_GEM_ATK_4,44;Item_GEM_DEF_1,11;Item_GEM_DEF_2,22;Item_GEM_DEF_3,33;Item_GEM_DEF_4,44;Item_GEM_DEF_5,55;Item_GEM_FIRE_1,11;Item_GEM_FIRE_2,22;Item_GEM_FIRE_3,33;Item_GEM_WIND_1,11;Item_GEM_WIND_2,22;Item_GEM_WIND_3,33;Item_HeroCard_Abaddon,88;Item_HeroCard_Beastmaster,99;Item_HeroCard_BountyHunter,66;Item_HeroCard_Bristleback,33;Item_HeroCard_Clinkz,66;Item_HeroCard_CrystalMaiden,99;Item_HeroCard_Ezalor,99;Item_HeroCard_Lifestealer,99;Item_HeroCard_TeaantProtector,99</t>
+  </si>
+  <si>
     <t>NameID_NoobPack</t>
   </si>
   <si>
@@ -753,76 +756,133 @@
     <t>Item_GEM_POISON_10</t>
   </si>
   <si>
-    <t>Item_HeroCard_1</t>
-  </si>
-  <si>
-    <t>Desc_HeroCard_1</t>
+    <t>Item_HeroCard_Abaddon</t>
+  </si>
+  <si>
+    <t>Desc_HeroCard_Abaddon</t>
   </si>
   <si>
     <t>Hero_1</t>
   </si>
   <si>
-    <t>NameID_HeroCard_1</t>
-  </si>
-  <si>
-    <t>Item_HeroCard_2</t>
-  </si>
-  <si>
-    <t>Desc_HeroCard_2</t>
+    <t>UIResources/Sprites/Hero</t>
+  </si>
+  <si>
+    <t>Hero_Abaddon</t>
+  </si>
+  <si>
+    <t>NameID_Abaddon</t>
+  </si>
+  <si>
+    <t>Item_HeroCard_Beastmaster</t>
+  </si>
+  <si>
+    <t>Desc_HeroCard_Beastmaster</t>
   </si>
   <si>
     <t>Hero_2</t>
   </si>
   <si>
-    <t>NameID_HeroCard_2</t>
-  </si>
-  <si>
-    <t>Item_HeroCard_3</t>
-  </si>
-  <si>
-    <t>Desc_HeroCard_3</t>
+    <t>Hero_Beastmaster</t>
+  </si>
+  <si>
+    <t>NameID_Beastmaster</t>
+  </si>
+  <si>
+    <t>Item_HeroCard_BountyHunter</t>
+  </si>
+  <si>
+    <t>Desc_HeroCard_BountyHunter</t>
   </si>
   <si>
     <t>Hero_3</t>
   </si>
   <si>
-    <t>NameID_HeroCard_3</t>
-  </si>
-  <si>
-    <t>Item_HeroCard_4</t>
-  </si>
-  <si>
-    <t>Desc_HeroCard_4</t>
+    <t>Hero_BountyHunter</t>
+  </si>
+  <si>
+    <t>NameID_BountyHunter</t>
+  </si>
+  <si>
+    <t>Item_HeroCard_Bristleback</t>
+  </si>
+  <si>
+    <t>Desc_HeroCard_Bristleback</t>
   </si>
   <si>
     <t>Hero_4</t>
   </si>
   <si>
-    <t>NameID_HeroCard_4</t>
-  </si>
-  <si>
-    <t>Item_HeroCard_5</t>
-  </si>
-  <si>
-    <t>Desc_HeroCard_5</t>
+    <t>Hero_Bristleback</t>
+  </si>
+  <si>
+    <t>NameID_Bristleback</t>
+  </si>
+  <si>
+    <t>Item_HeroCard_Clinkz</t>
+  </si>
+  <si>
+    <t>Desc_HeroCard_Clinkz</t>
   </si>
   <si>
     <t>Hero_5</t>
   </si>
   <si>
-    <t>NameID_HeroCard_5</t>
-  </si>
-  <si>
-    <t>Item_HeroCard_6</t>
-  </si>
-  <si>
-    <t>Desc_HeroCard_6</t>
+    <t>Hero_Clinkz</t>
+  </si>
+  <si>
+    <t>NameID_Clinkz</t>
+  </si>
+  <si>
+    <t>Item_HeroCard_CrystalMaiden</t>
+  </si>
+  <si>
+    <t>Desc_HeroCard_CrystalMaiden</t>
   </si>
   <si>
     <t>Hero_6</t>
   </si>
   <si>
-    <t>NameID_HeroCard_6</t>
+    <t>Hero_CrystalMaiden</t>
+  </si>
+  <si>
+    <t>NameID_CrystalMaiden</t>
+  </si>
+  <si>
+    <t>Item_HeroCard_Ezalor</t>
+  </si>
+  <si>
+    <t>Desc_HeroCard_Ezalor</t>
+  </si>
+  <si>
+    <t>Hero_Ezalor</t>
+  </si>
+  <si>
+    <t>NameID_Ezalor</t>
+  </si>
+  <si>
+    <t>Item_HeroCard_Lifestealer</t>
+  </si>
+  <si>
+    <t>Desc_HeroCard_Lifestealer</t>
+  </si>
+  <si>
+    <t>Hero_Lifestealer</t>
+  </si>
+  <si>
+    <t>NameID_Lifestealer</t>
+  </si>
+  <si>
+    <t>Item_HeroCard_TeaantProtector</t>
+  </si>
+  <si>
+    <t>Desc_HeroCard_TeaantProtector</t>
+  </si>
+  <si>
+    <t>Hero_TeaantProtector</t>
+  </si>
+  <si>
+    <t>NameID_TeaantProtector</t>
   </si>
 </sst>
 </file>
@@ -830,9 +890,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22">
@@ -860,16 +920,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -889,9 +950,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -906,14 +966,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -927,16 +980,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -950,14 +996,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -965,9 +1003,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -990,7 +1050,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1003,7 +1063,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1030,7 +1090,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399945066682943"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1042,7 +1102,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1054,7 +1150,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1066,25 +1192,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1096,7 +1228,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1108,7 +1246,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1120,79 +1258,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1204,7 +1270,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1293,6 +1359,15 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1328,6 +1403,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1347,51 +1452,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1409,130 +1475,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1679,7 +1745,7 @@
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="1">
     <dxf>
       <font>
         <b val="1"/>
@@ -1690,11 +1756,9 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf/>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2">
-    <tableStyle name="MySqlDefault" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
+    <tableStyle name="MySqlDefault" count="1">
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
@@ -1959,14 +2023,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:V137"/>
+  <dimension ref="A1:V140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="M125" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="G40" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="S11" sqref="S11:S137"/>
+      <selection pane="bottomRight" activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1988,8 +2052,7 @@
     <col min="16" max="16" width="12.6637168141593" customWidth="1"/>
     <col min="17" max="17" width="14" customWidth="1"/>
     <col min="18" max="18" width="18.6637168141593" customWidth="1"/>
-    <col min="19" max="19" width="23.3362831858407" customWidth="1"/>
-    <col min="20" max="20" width="23.3362831858407" customWidth="1"/>
+    <col min="19" max="20" width="23.3362831858407" customWidth="1"/>
     <col min="21" max="21" width="21.5044247787611" customWidth="1"/>
     <col min="22" max="22" width="8.66371681415929" customWidth="1"/>
   </cols>
@@ -4643,7 +4706,7 @@
         <v>0</v>
       </c>
       <c r="D46" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46" s="17"/>
       <c r="F46" s="17">
@@ -4654,7 +4717,9 @@
       </c>
       <c r="H46" s="17"/>
       <c r="I46" s="17"/>
-      <c r="J46" s="17"/>
+      <c r="J46" s="17" t="s">
+        <v>140</v>
+      </c>
       <c r="K46" s="17">
         <v>0</v>
       </c>
@@ -4682,7 +4747,7 @@
         <v>138</v>
       </c>
       <c r="U46" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="V46" s="17">
         <v>0</v>
@@ -4690,7 +4755,7 @@
     </row>
     <row r="47" s="5" customFormat="1" spans="1:22">
       <c r="A47" s="16" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B47" s="18">
         <v>5</v>
@@ -4735,10 +4800,10 @@
         <v>56</v>
       </c>
       <c r="T47" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="U47" s="16" t="s">
         <v>141</v>
-      </c>
-      <c r="U47" s="16" t="s">
-        <v>140</v>
       </c>
       <c r="V47" s="17">
         <v>0</v>
@@ -4746,7 +4811,7 @@
     </row>
     <row r="48" s="5" customFormat="1" spans="1:22">
       <c r="A48" s="16" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B48" s="17">
         <v>5</v>
@@ -4791,10 +4856,10 @@
         <v>56</v>
       </c>
       <c r="T48" s="16" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="U48" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="V48" s="17">
         <v>0</v>
@@ -4802,7 +4867,7 @@
     </row>
     <row r="49" s="5" customFormat="1" spans="1:22">
       <c r="A49" s="16" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B49" s="18">
         <v>5</v>
@@ -4847,10 +4912,10 @@
         <v>56</v>
       </c>
       <c r="T49" s="16" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="U49" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="V49" s="17">
         <v>0</v>
@@ -4858,7 +4923,7 @@
     </row>
     <row r="50" s="5" customFormat="1" spans="1:22">
       <c r="A50" s="16" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B50" s="17">
         <v>5</v>
@@ -4903,10 +4968,10 @@
         <v>56</v>
       </c>
       <c r="T50" s="16" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="U50" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="V50" s="17">
         <v>0</v>
@@ -4914,7 +4979,7 @@
     </row>
     <row r="51" s="5" customFormat="1" spans="1:22">
       <c r="A51" s="16" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B51" s="18">
         <v>5</v>
@@ -4959,10 +5024,10 @@
         <v>56</v>
       </c>
       <c r="T51" s="16" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="U51" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="V51" s="17">
         <v>0</v>
@@ -4970,7 +5035,7 @@
     </row>
     <row r="52" s="5" customFormat="1" spans="1:22">
       <c r="A52" s="16" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B52" s="17">
         <v>5</v>
@@ -5015,10 +5080,10 @@
         <v>56</v>
       </c>
       <c r="T52" s="16" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="U52" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="V52" s="17">
         <v>0</v>
@@ -5026,7 +5091,7 @@
     </row>
     <row r="53" s="5" customFormat="1" spans="1:22">
       <c r="A53" s="16" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B53" s="18">
         <v>5</v>
@@ -5071,10 +5136,10 @@
         <v>56</v>
       </c>
       <c r="T53" s="16" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="U53" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="V53" s="17">
         <v>0</v>
@@ -5082,7 +5147,7 @@
     </row>
     <row r="54" s="5" customFormat="1" spans="1:22">
       <c r="A54" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B54" s="17">
         <v>5</v>
@@ -5127,10 +5192,10 @@
         <v>56</v>
       </c>
       <c r="T54" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="U54" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="V54" s="17">
         <v>0</v>
@@ -5138,7 +5203,7 @@
     </row>
     <row r="55" s="5" customFormat="1" spans="1:22">
       <c r="A55" s="16" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B55" s="18">
         <v>5</v>
@@ -5183,10 +5248,10 @@
         <v>56</v>
       </c>
       <c r="T55" s="16" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="U55" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="V55" s="17">
         <v>0</v>
@@ -5194,7 +5259,7 @@
     </row>
     <row r="56" s="5" customFormat="1" spans="1:22">
       <c r="A56" s="16" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B56" s="17">
         <v>5</v>
@@ -5210,7 +5275,7 @@
         <v>0</v>
       </c>
       <c r="G56" s="16" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H56" s="17"/>
       <c r="I56" s="17"/>
@@ -5239,10 +5304,10 @@
         <v>56</v>
       </c>
       <c r="T56" s="16" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="U56" s="16" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="V56" s="17">
         <v>0</v>
@@ -5250,7 +5315,7 @@
     </row>
     <row r="57" s="5" customFormat="1" spans="1:22">
       <c r="A57" s="16" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B57" s="18">
         <v>5</v>
@@ -5266,7 +5331,7 @@
         <v>0</v>
       </c>
       <c r="G57" s="16" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H57" s="17"/>
       <c r="I57" s="17"/>
@@ -5295,10 +5360,10 @@
         <v>56</v>
       </c>
       <c r="T57" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="U57" s="16" t="s">
         <v>153</v>
-      </c>
-      <c r="U57" s="16" t="s">
-        <v>152</v>
       </c>
       <c r="V57" s="17">
         <v>0</v>
@@ -5306,7 +5371,7 @@
     </row>
     <row r="58" s="5" customFormat="1" spans="1:22">
       <c r="A58" s="16" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B58" s="17">
         <v>5</v>
@@ -5322,7 +5387,7 @@
         <v>0</v>
       </c>
       <c r="G58" s="16" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H58" s="17"/>
       <c r="I58" s="17"/>
@@ -5351,10 +5416,10 @@
         <v>56</v>
       </c>
       <c r="T58" s="16" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="U58" s="16" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="V58" s="17">
         <v>0</v>
@@ -5362,7 +5427,7 @@
     </row>
     <row r="59" s="5" customFormat="1" spans="1:22">
       <c r="A59" s="16" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B59" s="18">
         <v>5</v>
@@ -5378,7 +5443,7 @@
         <v>0</v>
       </c>
       <c r="G59" s="16" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H59" s="17"/>
       <c r="I59" s="17"/>
@@ -5407,10 +5472,10 @@
         <v>56</v>
       </c>
       <c r="T59" s="16" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="U59" s="16" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="V59" s="17">
         <v>0</v>
@@ -5418,7 +5483,7 @@
     </row>
     <row r="60" s="5" customFormat="1" spans="1:22">
       <c r="A60" s="19" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B60" s="17">
         <v>5</v>
@@ -5434,7 +5499,7 @@
         <v>0</v>
       </c>
       <c r="G60" s="16" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H60" s="20"/>
       <c r="I60" s="20"/>
@@ -5463,10 +5528,10 @@
         <v>56</v>
       </c>
       <c r="T60" s="19" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="U60" s="16" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="V60" s="20">
         <v>0</v>
@@ -5474,7 +5539,7 @@
     </row>
     <row r="61" s="5" customFormat="1" spans="1:22">
       <c r="A61" s="19" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B61" s="17">
         <v>5</v>
@@ -5490,7 +5555,7 @@
         <v>0</v>
       </c>
       <c r="G61" s="16" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H61" s="20"/>
       <c r="I61" s="20"/>
@@ -5519,10 +5584,10 @@
         <v>56</v>
       </c>
       <c r="T61" s="19" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="U61" s="16" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="V61" s="20">
         <v>0</v>
@@ -5530,7 +5595,7 @@
     </row>
     <row r="62" s="6" customFormat="1" spans="1:22">
       <c r="A62" s="22" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B62" s="22">
         <v>1</v>
@@ -5546,7 +5611,7 @@
         <v>1</v>
       </c>
       <c r="G62" s="22" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H62" s="22"/>
       <c r="I62" s="22"/>
@@ -5575,10 +5640,10 @@
         <v>56</v>
       </c>
       <c r="T62" s="22" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="U62" s="22" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="V62" s="22">
         <v>0</v>
@@ -5586,7 +5651,7 @@
     </row>
     <row r="63" s="6" customFormat="1" spans="1:22">
       <c r="A63" s="22" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B63" s="22">
         <v>1</v>
@@ -5602,7 +5667,7 @@
         <v>2</v>
       </c>
       <c r="G63" s="22" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H63" s="22"/>
       <c r="I63" s="22"/>
@@ -5631,10 +5696,10 @@
         <v>56</v>
       </c>
       <c r="T63" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="U63" s="22" t="s">
         <v>161</v>
-      </c>
-      <c r="U63" s="22" t="s">
-        <v>160</v>
       </c>
       <c r="V63" s="22">
         <v>0</v>
@@ -5642,7 +5707,7 @@
     </row>
     <row r="64" s="6" customFormat="1" spans="1:22">
       <c r="A64" s="22" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B64" s="22">
         <v>1</v>
@@ -5658,7 +5723,7 @@
         <v>3</v>
       </c>
       <c r="G64" s="22" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H64" s="22"/>
       <c r="I64" s="22"/>
@@ -5687,10 +5752,10 @@
         <v>56</v>
       </c>
       <c r="T64" s="22" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="U64" s="22" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="V64" s="22">
         <v>0</v>
@@ -5698,7 +5763,7 @@
     </row>
     <row r="65" s="6" customFormat="1" spans="1:22">
       <c r="A65" s="22" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B65" s="22">
         <v>1</v>
@@ -5714,7 +5779,7 @@
         <v>4</v>
       </c>
       <c r="G65" s="22" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H65" s="22"/>
       <c r="I65" s="22"/>
@@ -5743,10 +5808,10 @@
         <v>56</v>
       </c>
       <c r="T65" s="22" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="U65" s="22" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="V65" s="22">
         <v>0</v>
@@ -5754,7 +5819,7 @@
     </row>
     <row r="66" s="6" customFormat="1" spans="1:22">
       <c r="A66" s="22" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B66" s="22">
         <v>1</v>
@@ -5770,7 +5835,7 @@
         <v>5</v>
       </c>
       <c r="G66" s="22" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H66" s="22"/>
       <c r="I66" s="22"/>
@@ -5799,10 +5864,10 @@
         <v>56</v>
       </c>
       <c r="T66" s="22" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="U66" s="22" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="V66" s="22">
         <v>0</v>
@@ -5810,7 +5875,7 @@
     </row>
     <row r="67" s="6" customFormat="1" spans="1:22">
       <c r="A67" s="22" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B67" s="22">
         <v>1</v>
@@ -5826,7 +5891,7 @@
         <v>6</v>
       </c>
       <c r="G67" s="22" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H67" s="22"/>
       <c r="I67" s="22"/>
@@ -5855,10 +5920,10 @@
         <v>56</v>
       </c>
       <c r="T67" s="22" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="U67" s="22" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="V67" s="22">
         <v>0</v>
@@ -5866,7 +5931,7 @@
     </row>
     <row r="68" s="6" customFormat="1" spans="1:22">
       <c r="A68" s="22" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B68" s="22">
         <v>1</v>
@@ -5882,7 +5947,7 @@
         <v>7</v>
       </c>
       <c r="G68" s="22" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H68" s="22"/>
       <c r="I68" s="22"/>
@@ -5911,10 +5976,10 @@
         <v>56</v>
       </c>
       <c r="T68" s="22" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="U68" s="22" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="V68" s="22">
         <v>0</v>
@@ -5922,7 +5987,7 @@
     </row>
     <row r="69" s="6" customFormat="1" spans="1:22">
       <c r="A69" s="22" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B69" s="22">
         <v>1</v>
@@ -5938,7 +6003,7 @@
         <v>8</v>
       </c>
       <c r="G69" s="22" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H69" s="22"/>
       <c r="I69" s="22"/>
@@ -5967,10 +6032,10 @@
         <v>56</v>
       </c>
       <c r="T69" s="22" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="U69" s="22" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="V69" s="22">
         <v>0</v>
@@ -5978,7 +6043,7 @@
     </row>
     <row r="70" s="6" customFormat="1" spans="1:22">
       <c r="A70" s="22" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B70" s="22">
         <v>1</v>
@@ -5994,7 +6059,7 @@
         <v>9</v>
       </c>
       <c r="G70" s="22" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H70" s="22"/>
       <c r="I70" s="22"/>
@@ -6023,10 +6088,10 @@
         <v>56</v>
       </c>
       <c r="T70" s="22" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="U70" s="22" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="V70" s="22">
         <v>0</v>
@@ -6034,7 +6099,7 @@
     </row>
     <row r="71" s="6" customFormat="1" spans="1:22">
       <c r="A71" s="22" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B71" s="22">
         <v>1</v>
@@ -6050,7 +6115,7 @@
         <v>10</v>
       </c>
       <c r="G71" s="22" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H71" s="22"/>
       <c r="I71" s="22"/>
@@ -6079,10 +6144,10 @@
         <v>56</v>
       </c>
       <c r="T71" s="22" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="U71" s="22" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="V71" s="22">
         <v>0</v>
@@ -6090,7 +6155,7 @@
     </row>
     <row r="72" s="6" customFormat="1" spans="1:22">
       <c r="A72" s="22" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B72" s="22">
         <v>1</v>
@@ -6106,7 +6171,7 @@
         <v>1</v>
       </c>
       <c r="G72" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H72" s="22"/>
       <c r="I72" s="22"/>
@@ -6135,10 +6200,10 @@
         <v>56</v>
       </c>
       <c r="T72" s="22" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="U72" s="22" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="V72" s="22">
         <v>0</v>
@@ -6146,7 +6211,7 @@
     </row>
     <row r="73" s="6" customFormat="1" spans="1:22">
       <c r="A73" s="22" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B73" s="22">
         <v>1</v>
@@ -6162,7 +6227,7 @@
         <v>2</v>
       </c>
       <c r="G73" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H73" s="22"/>
       <c r="I73" s="22"/>
@@ -6191,10 +6256,10 @@
         <v>56</v>
       </c>
       <c r="T73" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="U73" s="22" t="s">
         <v>173</v>
-      </c>
-      <c r="U73" s="22" t="s">
-        <v>172</v>
       </c>
       <c r="V73" s="22">
         <v>0</v>
@@ -6202,7 +6267,7 @@
     </row>
     <row r="74" s="6" customFormat="1" spans="1:22">
       <c r="A74" s="22" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B74" s="22">
         <v>1</v>
@@ -6218,7 +6283,7 @@
         <v>3</v>
       </c>
       <c r="G74" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H74" s="22"/>
       <c r="I74" s="22"/>
@@ -6247,10 +6312,10 @@
         <v>56</v>
       </c>
       <c r="T74" s="22" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="U74" s="22" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="V74" s="22">
         <v>0</v>
@@ -6258,7 +6323,7 @@
     </row>
     <row r="75" s="6" customFormat="1" spans="1:22">
       <c r="A75" s="22" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B75" s="22">
         <v>1</v>
@@ -6274,7 +6339,7 @@
         <v>4</v>
       </c>
       <c r="G75" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H75" s="22"/>
       <c r="I75" s="22"/>
@@ -6303,10 +6368,10 @@
         <v>56</v>
       </c>
       <c r="T75" s="22" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="U75" s="22" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="V75" s="22">
         <v>0</v>
@@ -6314,7 +6379,7 @@
     </row>
     <row r="76" s="6" customFormat="1" spans="1:22">
       <c r="A76" s="22" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B76" s="22">
         <v>1</v>
@@ -6330,7 +6395,7 @@
         <v>5</v>
       </c>
       <c r="G76" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H76" s="22"/>
       <c r="I76" s="22"/>
@@ -6359,10 +6424,10 @@
         <v>56</v>
       </c>
       <c r="T76" s="22" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="U76" s="22" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="V76" s="22">
         <v>0</v>
@@ -6370,7 +6435,7 @@
     </row>
     <row r="77" s="6" customFormat="1" spans="1:22">
       <c r="A77" s="22" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B77" s="22">
         <v>1</v>
@@ -6386,7 +6451,7 @@
         <v>6</v>
       </c>
       <c r="G77" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H77" s="22"/>
       <c r="I77" s="22"/>
@@ -6415,10 +6480,10 @@
         <v>56</v>
       </c>
       <c r="T77" s="22" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="U77" s="22" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="V77" s="22">
         <v>0</v>
@@ -6426,7 +6491,7 @@
     </row>
     <row r="78" s="6" customFormat="1" spans="1:22">
       <c r="A78" s="22" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B78" s="22">
         <v>1</v>
@@ -6442,7 +6507,7 @@
         <v>7</v>
       </c>
       <c r="G78" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H78" s="22"/>
       <c r="I78" s="22"/>
@@ -6471,10 +6536,10 @@
         <v>56</v>
       </c>
       <c r="T78" s="22" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="U78" s="22" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="V78" s="22">
         <v>0</v>
@@ -6482,7 +6547,7 @@
     </row>
     <row r="79" s="6" customFormat="1" spans="1:22">
       <c r="A79" s="22" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B79" s="22">
         <v>1</v>
@@ -6498,7 +6563,7 @@
         <v>8</v>
       </c>
       <c r="G79" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H79" s="22"/>
       <c r="I79" s="22"/>
@@ -6527,10 +6592,10 @@
         <v>56</v>
       </c>
       <c r="T79" s="22" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U79" s="22" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="V79" s="22">
         <v>0</v>
@@ -6538,7 +6603,7 @@
     </row>
     <row r="80" s="6" customFormat="1" spans="1:22">
       <c r="A80" s="22" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B80" s="22">
         <v>1</v>
@@ -6554,7 +6619,7 @@
         <v>9</v>
       </c>
       <c r="G80" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H80" s="22"/>
       <c r="I80" s="22"/>
@@ -6583,10 +6648,10 @@
         <v>56</v>
       </c>
       <c r="T80" s="22" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U80" s="22" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="V80" s="22">
         <v>0</v>
@@ -6594,7 +6659,7 @@
     </row>
     <row r="81" s="6" customFormat="1" spans="1:22">
       <c r="A81" s="22" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B81" s="22">
         <v>1</v>
@@ -6610,7 +6675,7 @@
         <v>10</v>
       </c>
       <c r="G81" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H81" s="22"/>
       <c r="I81" s="22"/>
@@ -6639,10 +6704,10 @@
         <v>56</v>
       </c>
       <c r="T81" s="22" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="U81" s="22" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="V81" s="22">
         <v>0</v>
@@ -6650,7 +6715,7 @@
     </row>
     <row r="82" s="6" customFormat="1" spans="1:22">
       <c r="A82" s="22" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B82" s="22">
         <v>1</v>
@@ -6666,7 +6731,7 @@
         <v>1</v>
       </c>
       <c r="G82" s="22" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H82" s="22"/>
       <c r="I82" s="22"/>
@@ -6695,10 +6760,10 @@
         <v>56</v>
       </c>
       <c r="T82" s="22" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="U82" s="22" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="V82" s="22">
         <v>0</v>
@@ -6706,7 +6771,7 @@
     </row>
     <row r="83" s="6" customFormat="1" spans="1:22">
       <c r="A83" s="22" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B83" s="22">
         <v>1</v>
@@ -6722,7 +6787,7 @@
         <v>2</v>
       </c>
       <c r="G83" s="22" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H83" s="22"/>
       <c r="I83" s="22"/>
@@ -6751,10 +6816,10 @@
         <v>56</v>
       </c>
       <c r="T83" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="U83" s="22" t="s">
         <v>185</v>
-      </c>
-      <c r="U83" s="22" t="s">
-        <v>184</v>
       </c>
       <c r="V83" s="22">
         <v>0</v>
@@ -6762,7 +6827,7 @@
     </row>
     <row r="84" s="6" customFormat="1" spans="1:22">
       <c r="A84" s="22" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B84" s="22">
         <v>1</v>
@@ -6778,7 +6843,7 @@
         <v>3</v>
       </c>
       <c r="G84" s="22" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H84" s="22"/>
       <c r="I84" s="22"/>
@@ -6807,10 +6872,10 @@
         <v>56</v>
       </c>
       <c r="T84" s="22" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="U84" s="22" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="V84" s="22">
         <v>0</v>
@@ -6818,7 +6883,7 @@
     </row>
     <row r="85" s="6" customFormat="1" spans="1:22">
       <c r="A85" s="22" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B85" s="22">
         <v>1</v>
@@ -6834,7 +6899,7 @@
         <v>4</v>
       </c>
       <c r="G85" s="22" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H85" s="22"/>
       <c r="I85" s="22"/>
@@ -6863,10 +6928,10 @@
         <v>56</v>
       </c>
       <c r="T85" s="22" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="U85" s="22" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="V85" s="22">
         <v>0</v>
@@ -6874,7 +6939,7 @@
     </row>
     <row r="86" s="6" customFormat="1" spans="1:22">
       <c r="A86" s="22" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B86" s="22">
         <v>1</v>
@@ -6890,7 +6955,7 @@
         <v>5</v>
       </c>
       <c r="G86" s="22" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H86" s="22"/>
       <c r="I86" s="22"/>
@@ -6919,10 +6984,10 @@
         <v>56</v>
       </c>
       <c r="T86" s="22" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="U86" s="22" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="V86" s="22">
         <v>0</v>
@@ -6930,7 +6995,7 @@
     </row>
     <row r="87" s="6" customFormat="1" spans="1:22">
       <c r="A87" s="22" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B87" s="22">
         <v>1</v>
@@ -6946,7 +7011,7 @@
         <v>6</v>
       </c>
       <c r="G87" s="22" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H87" s="22"/>
       <c r="I87" s="22"/>
@@ -6975,10 +7040,10 @@
         <v>56</v>
       </c>
       <c r="T87" s="22" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="U87" s="22" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="V87" s="22">
         <v>0</v>
@@ -6986,7 +7051,7 @@
     </row>
     <row r="88" s="6" customFormat="1" spans="1:22">
       <c r="A88" s="22" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B88" s="22">
         <v>1</v>
@@ -7002,7 +7067,7 @@
         <v>7</v>
       </c>
       <c r="G88" s="22" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H88" s="22"/>
       <c r="I88" s="22"/>
@@ -7031,10 +7096,10 @@
         <v>56</v>
       </c>
       <c r="T88" s="22" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="U88" s="22" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="V88" s="22">
         <v>0</v>
@@ -7042,7 +7107,7 @@
     </row>
     <row r="89" s="6" customFormat="1" spans="1:22">
       <c r="A89" s="22" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B89" s="22">
         <v>1</v>
@@ -7058,7 +7123,7 @@
         <v>8</v>
       </c>
       <c r="G89" s="22" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H89" s="22"/>
       <c r="I89" s="22"/>
@@ -7087,10 +7152,10 @@
         <v>56</v>
       </c>
       <c r="T89" s="22" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="U89" s="22" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="V89" s="22">
         <v>0</v>
@@ -7098,7 +7163,7 @@
     </row>
     <row r="90" s="6" customFormat="1" spans="1:22">
       <c r="A90" s="22" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B90" s="22">
         <v>1</v>
@@ -7114,7 +7179,7 @@
         <v>9</v>
       </c>
       <c r="G90" s="22" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H90" s="22"/>
       <c r="I90" s="22"/>
@@ -7143,10 +7208,10 @@
         <v>56</v>
       </c>
       <c r="T90" s="22" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="U90" s="22" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="V90" s="22">
         <v>0</v>
@@ -7154,7 +7219,7 @@
     </row>
     <row r="91" s="6" customFormat="1" spans="1:22">
       <c r="A91" s="22" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B91" s="22">
         <v>1</v>
@@ -7170,7 +7235,7 @@
         <v>10</v>
       </c>
       <c r="G91" s="22" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H91" s="22"/>
       <c r="I91" s="22"/>
@@ -7199,10 +7264,10 @@
         <v>56</v>
       </c>
       <c r="T91" s="22" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="U91" s="22" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="V91" s="22">
         <v>0</v>
@@ -7210,7 +7275,7 @@
     </row>
     <row r="92" s="6" customFormat="1" spans="1:22">
       <c r="A92" s="22" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B92" s="22">
         <v>1</v>
@@ -7226,7 +7291,7 @@
         <v>1</v>
       </c>
       <c r="G92" s="22" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H92" s="22"/>
       <c r="I92" s="22"/>
@@ -7255,10 +7320,10 @@
         <v>56</v>
       </c>
       <c r="T92" s="22" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="U92" s="22" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="V92" s="22">
         <v>0</v>
@@ -7266,7 +7331,7 @@
     </row>
     <row r="93" s="6" customFormat="1" spans="1:22">
       <c r="A93" s="22" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B93" s="22">
         <v>1</v>
@@ -7282,7 +7347,7 @@
         <v>2</v>
       </c>
       <c r="G93" s="22" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H93" s="22"/>
       <c r="I93" s="22"/>
@@ -7311,10 +7376,10 @@
         <v>56</v>
       </c>
       <c r="T93" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="U93" s="22" t="s">
         <v>197</v>
-      </c>
-      <c r="U93" s="22" t="s">
-        <v>196</v>
       </c>
       <c r="V93" s="22">
         <v>0</v>
@@ -7322,7 +7387,7 @@
     </row>
     <row r="94" s="6" customFormat="1" spans="1:22">
       <c r="A94" s="22" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B94" s="22">
         <v>1</v>
@@ -7338,7 +7403,7 @@
         <v>3</v>
       </c>
       <c r="G94" s="22" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H94" s="22"/>
       <c r="I94" s="22"/>
@@ -7367,10 +7432,10 @@
         <v>56</v>
       </c>
       <c r="T94" s="22" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="U94" s="22" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="V94" s="22">
         <v>0</v>
@@ -7378,7 +7443,7 @@
     </row>
     <row r="95" s="6" customFormat="1" spans="1:22">
       <c r="A95" s="22" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B95" s="22">
         <v>1</v>
@@ -7394,7 +7459,7 @@
         <v>4</v>
       </c>
       <c r="G95" s="22" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H95" s="22"/>
       <c r="I95" s="22"/>
@@ -7423,10 +7488,10 @@
         <v>56</v>
       </c>
       <c r="T95" s="22" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="U95" s="22" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="V95" s="22">
         <v>0</v>
@@ -7434,7 +7499,7 @@
     </row>
     <row r="96" s="6" customFormat="1" spans="1:22">
       <c r="A96" s="22" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B96" s="22">
         <v>1</v>
@@ -7450,7 +7515,7 @@
         <v>5</v>
       </c>
       <c r="G96" s="22" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H96" s="22"/>
       <c r="I96" s="22"/>
@@ -7479,10 +7544,10 @@
         <v>56</v>
       </c>
       <c r="T96" s="22" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U96" s="22" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="V96" s="22">
         <v>0</v>
@@ -7490,7 +7555,7 @@
     </row>
     <row r="97" s="6" customFormat="1" spans="1:22">
       <c r="A97" s="22" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B97" s="22">
         <v>1</v>
@@ -7506,7 +7571,7 @@
         <v>6</v>
       </c>
       <c r="G97" s="22" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H97" s="22"/>
       <c r="I97" s="22"/>
@@ -7535,10 +7600,10 @@
         <v>56</v>
       </c>
       <c r="T97" s="22" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="U97" s="22" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="V97" s="22">
         <v>0</v>
@@ -7546,7 +7611,7 @@
     </row>
     <row r="98" s="6" customFormat="1" spans="1:22">
       <c r="A98" s="22" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B98" s="22">
         <v>1</v>
@@ -7562,7 +7627,7 @@
         <v>7</v>
       </c>
       <c r="G98" s="22" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H98" s="22"/>
       <c r="I98" s="22"/>
@@ -7591,10 +7656,10 @@
         <v>56</v>
       </c>
       <c r="T98" s="22" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="U98" s="22" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="V98" s="22">
         <v>0</v>
@@ -7602,7 +7667,7 @@
     </row>
     <row r="99" s="6" customFormat="1" spans="1:22">
       <c r="A99" s="22" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B99" s="22">
         <v>1</v>
@@ -7618,7 +7683,7 @@
         <v>8</v>
       </c>
       <c r="G99" s="22" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H99" s="22"/>
       <c r="I99" s="22"/>
@@ -7647,10 +7712,10 @@
         <v>56</v>
       </c>
       <c r="T99" s="22" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="U99" s="22" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="V99" s="22">
         <v>0</v>
@@ -7658,7 +7723,7 @@
     </row>
     <row r="100" s="6" customFormat="1" spans="1:22">
       <c r="A100" s="22" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B100" s="22">
         <v>1</v>
@@ -7674,7 +7739,7 @@
         <v>9</v>
       </c>
       <c r="G100" s="22" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H100" s="22"/>
       <c r="I100" s="22"/>
@@ -7703,10 +7768,10 @@
         <v>56</v>
       </c>
       <c r="T100" s="22" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="U100" s="22" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="V100" s="22">
         <v>0</v>
@@ -7714,7 +7779,7 @@
     </row>
     <row r="101" s="6" customFormat="1" spans="1:22">
       <c r="A101" s="22" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B101" s="22">
         <v>1</v>
@@ -7730,7 +7795,7 @@
         <v>10</v>
       </c>
       <c r="G101" s="22" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H101" s="22"/>
       <c r="I101" s="22"/>
@@ -7759,10 +7824,10 @@
         <v>56</v>
       </c>
       <c r="T101" s="22" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="U101" s="22" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="V101" s="22">
         <v>0</v>
@@ -7770,7 +7835,7 @@
     </row>
     <row r="102" s="7" customFormat="1" spans="1:22">
       <c r="A102" s="23" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B102" s="23">
         <v>1</v>
@@ -7786,7 +7851,7 @@
         <v>1</v>
       </c>
       <c r="G102" s="23" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H102" s="23"/>
       <c r="I102" s="23"/>
@@ -7815,10 +7880,10 @@
         <v>56</v>
       </c>
       <c r="T102" s="23" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="U102" s="23" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="V102" s="23">
         <v>0</v>
@@ -7826,7 +7891,7 @@
     </row>
     <row r="103" s="7" customFormat="1" spans="1:22">
       <c r="A103" s="23" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B103" s="23">
         <v>1</v>
@@ -7842,7 +7907,7 @@
         <v>2</v>
       </c>
       <c r="G103" s="23" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H103" s="23"/>
       <c r="I103" s="23"/>
@@ -7871,10 +7936,10 @@
         <v>56</v>
       </c>
       <c r="T103" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="U103" s="23" t="s">
         <v>209</v>
-      </c>
-      <c r="U103" s="23" t="s">
-        <v>208</v>
       </c>
       <c r="V103" s="23">
         <v>0</v>
@@ -7882,7 +7947,7 @@
     </row>
     <row r="104" s="7" customFormat="1" spans="1:22">
       <c r="A104" s="23" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B104" s="23">
         <v>1</v>
@@ -7898,7 +7963,7 @@
         <v>3</v>
       </c>
       <c r="G104" s="23" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H104" s="23"/>
       <c r="I104" s="23"/>
@@ -7927,10 +7992,10 @@
         <v>56</v>
       </c>
       <c r="T104" s="23" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="U104" s="23" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="V104" s="23">
         <v>0</v>
@@ -7938,7 +8003,7 @@
     </row>
     <row r="105" s="7" customFormat="1" spans="1:22">
       <c r="A105" s="23" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B105" s="23">
         <v>1</v>
@@ -7954,7 +8019,7 @@
         <v>4</v>
       </c>
       <c r="G105" s="23" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H105" s="23"/>
       <c r="I105" s="23"/>
@@ -7983,10 +8048,10 @@
         <v>56</v>
       </c>
       <c r="T105" s="23" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="U105" s="23" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="V105" s="23">
         <v>0</v>
@@ -7994,7 +8059,7 @@
     </row>
     <row r="106" s="7" customFormat="1" spans="1:22">
       <c r="A106" s="23" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B106" s="23">
         <v>1</v>
@@ -8010,7 +8075,7 @@
         <v>5</v>
       </c>
       <c r="G106" s="23" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H106" s="23"/>
       <c r="I106" s="23"/>
@@ -8039,10 +8104,10 @@
         <v>56</v>
       </c>
       <c r="T106" s="23" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="U106" s="23" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="V106" s="23">
         <v>0</v>
@@ -8050,7 +8115,7 @@
     </row>
     <row r="107" s="7" customFormat="1" spans="1:22">
       <c r="A107" s="23" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B107" s="23">
         <v>1</v>
@@ -8066,7 +8131,7 @@
         <v>6</v>
       </c>
       <c r="G107" s="23" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H107" s="23"/>
       <c r="I107" s="23"/>
@@ -8095,10 +8160,10 @@
         <v>56</v>
       </c>
       <c r="T107" s="23" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="U107" s="23" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="V107" s="23">
         <v>0</v>
@@ -8106,7 +8171,7 @@
     </row>
     <row r="108" s="7" customFormat="1" spans="1:22">
       <c r="A108" s="23" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B108" s="23">
         <v>1</v>
@@ -8122,7 +8187,7 @@
         <v>7</v>
       </c>
       <c r="G108" s="23" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H108" s="23"/>
       <c r="I108" s="23"/>
@@ -8151,10 +8216,10 @@
         <v>56</v>
       </c>
       <c r="T108" s="23" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="U108" s="23" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="V108" s="23">
         <v>0</v>
@@ -8162,7 +8227,7 @@
     </row>
     <row r="109" s="7" customFormat="1" spans="1:22">
       <c r="A109" s="23" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B109" s="23">
         <v>1</v>
@@ -8178,7 +8243,7 @@
         <v>8</v>
       </c>
       <c r="G109" s="23" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H109" s="23"/>
       <c r="I109" s="23"/>
@@ -8207,10 +8272,10 @@
         <v>56</v>
       </c>
       <c r="T109" s="23" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="U109" s="23" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="V109" s="23">
         <v>0</v>
@@ -8218,7 +8283,7 @@
     </row>
     <row r="110" s="7" customFormat="1" spans="1:22">
       <c r="A110" s="23" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B110" s="23">
         <v>1</v>
@@ -8234,7 +8299,7 @@
         <v>9</v>
       </c>
       <c r="G110" s="23" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H110" s="23"/>
       <c r="I110" s="23"/>
@@ -8263,10 +8328,10 @@
         <v>56</v>
       </c>
       <c r="T110" s="23" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="U110" s="23" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="V110" s="23">
         <v>0</v>
@@ -8274,7 +8339,7 @@
     </row>
     <row r="111" s="7" customFormat="1" spans="1:22">
       <c r="A111" s="23" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B111" s="23">
         <v>1</v>
@@ -8290,7 +8355,7 @@
         <v>10</v>
       </c>
       <c r="G111" s="23" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H111" s="23"/>
       <c r="I111" s="23"/>
@@ -8319,10 +8384,10 @@
         <v>56</v>
       </c>
       <c r="T111" s="23" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="U111" s="23" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="V111" s="23">
         <v>0</v>
@@ -8330,7 +8395,7 @@
     </row>
     <row r="112" s="6" customFormat="1" spans="1:22">
       <c r="A112" s="22" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B112" s="22">
         <v>1</v>
@@ -8346,7 +8411,7 @@
         <v>1</v>
       </c>
       <c r="G112" s="22" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H112" s="22"/>
       <c r="I112" s="22"/>
@@ -8375,10 +8440,10 @@
         <v>56</v>
       </c>
       <c r="T112" s="22" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="U112" s="22" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="V112" s="22">
         <v>0</v>
@@ -8386,7 +8451,7 @@
     </row>
     <row r="113" s="6" customFormat="1" spans="1:22">
       <c r="A113" s="22" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B113" s="22">
         <v>1</v>
@@ -8402,7 +8467,7 @@
         <v>2</v>
       </c>
       <c r="G113" s="22" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H113" s="22"/>
       <c r="I113" s="22"/>
@@ -8431,10 +8496,10 @@
         <v>56</v>
       </c>
       <c r="T113" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="U113" s="22" t="s">
         <v>221</v>
-      </c>
-      <c r="U113" s="22" t="s">
-        <v>220</v>
       </c>
       <c r="V113" s="22">
         <v>0</v>
@@ -8442,7 +8507,7 @@
     </row>
     <row r="114" s="6" customFormat="1" spans="1:22">
       <c r="A114" s="22" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B114" s="22">
         <v>1</v>
@@ -8458,7 +8523,7 @@
         <v>3</v>
       </c>
       <c r="G114" s="22" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H114" s="22"/>
       <c r="I114" s="22"/>
@@ -8487,10 +8552,10 @@
         <v>56</v>
       </c>
       <c r="T114" s="22" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="U114" s="22" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="V114" s="22">
         <v>0</v>
@@ -8498,7 +8563,7 @@
     </row>
     <row r="115" s="6" customFormat="1" spans="1:22">
       <c r="A115" s="22" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B115" s="22">
         <v>1</v>
@@ -8514,7 +8579,7 @@
         <v>4</v>
       </c>
       <c r="G115" s="22" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H115" s="22"/>
       <c r="I115" s="22"/>
@@ -8543,10 +8608,10 @@
         <v>56</v>
       </c>
       <c r="T115" s="22" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="U115" s="22" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="V115" s="22">
         <v>0</v>
@@ -8554,7 +8619,7 @@
     </row>
     <row r="116" s="6" customFormat="1" spans="1:22">
       <c r="A116" s="22" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B116" s="22">
         <v>1</v>
@@ -8570,7 +8635,7 @@
         <v>5</v>
       </c>
       <c r="G116" s="22" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H116" s="22"/>
       <c r="I116" s="22"/>
@@ -8599,10 +8664,10 @@
         <v>56</v>
       </c>
       <c r="T116" s="22" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="U116" s="22" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="V116" s="22">
         <v>0</v>
@@ -8610,7 +8675,7 @@
     </row>
     <row r="117" s="6" customFormat="1" spans="1:22">
       <c r="A117" s="22" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B117" s="22">
         <v>1</v>
@@ -8626,7 +8691,7 @@
         <v>6</v>
       </c>
       <c r="G117" s="22" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H117" s="22"/>
       <c r="I117" s="22"/>
@@ -8655,10 +8720,10 @@
         <v>56</v>
       </c>
       <c r="T117" s="22" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="U117" s="22" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="V117" s="22">
         <v>0</v>
@@ -8666,7 +8731,7 @@
     </row>
     <row r="118" s="6" customFormat="1" spans="1:22">
       <c r="A118" s="22" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B118" s="22">
         <v>1</v>
@@ -8682,7 +8747,7 @@
         <v>7</v>
       </c>
       <c r="G118" s="22" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H118" s="22"/>
       <c r="I118" s="22"/>
@@ -8711,10 +8776,10 @@
         <v>56</v>
       </c>
       <c r="T118" s="22" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="U118" s="22" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="V118" s="22">
         <v>0</v>
@@ -8722,7 +8787,7 @@
     </row>
     <row r="119" s="6" customFormat="1" spans="1:22">
       <c r="A119" s="22" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B119" s="22">
         <v>1</v>
@@ -8738,7 +8803,7 @@
         <v>8</v>
       </c>
       <c r="G119" s="22" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H119" s="22"/>
       <c r="I119" s="22"/>
@@ -8767,10 +8832,10 @@
         <v>56</v>
       </c>
       <c r="T119" s="22" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="U119" s="22" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="V119" s="22">
         <v>0</v>
@@ -8778,7 +8843,7 @@
     </row>
     <row r="120" s="6" customFormat="1" spans="1:22">
       <c r="A120" s="22" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B120" s="22">
         <v>1</v>
@@ -8794,7 +8859,7 @@
         <v>9</v>
       </c>
       <c r="G120" s="22" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H120" s="22"/>
       <c r="I120" s="22"/>
@@ -8823,10 +8888,10 @@
         <v>56</v>
       </c>
       <c r="T120" s="22" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="U120" s="22" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="V120" s="22">
         <v>0</v>
@@ -8834,7 +8899,7 @@
     </row>
     <row r="121" s="6" customFormat="1" spans="1:22">
       <c r="A121" s="22" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B121" s="22">
         <v>1</v>
@@ -8850,7 +8915,7 @@
         <v>10</v>
       </c>
       <c r="G121" s="22" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H121" s="22"/>
       <c r="I121" s="22"/>
@@ -8879,10 +8944,10 @@
         <v>56</v>
       </c>
       <c r="T121" s="22" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="U121" s="22" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="V121" s="22">
         <v>0</v>
@@ -8890,7 +8955,7 @@
     </row>
     <row r="122" s="6" customFormat="1" spans="1:22">
       <c r="A122" s="22" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B122" s="22">
         <v>1</v>
@@ -8906,7 +8971,7 @@
         <v>1</v>
       </c>
       <c r="G122" s="22" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H122" s="22"/>
       <c r="I122" s="22"/>
@@ -8935,10 +9000,10 @@
         <v>56</v>
       </c>
       <c r="T122" s="22" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="U122" s="22" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="V122" s="22">
         <v>0</v>
@@ -8946,7 +9011,7 @@
     </row>
     <row r="123" s="6" customFormat="1" spans="1:22">
       <c r="A123" s="22" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B123" s="22">
         <v>1</v>
@@ -8962,7 +9027,7 @@
         <v>2</v>
       </c>
       <c r="G123" s="22" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H123" s="22"/>
       <c r="I123" s="22"/>
@@ -8991,10 +9056,10 @@
         <v>56</v>
       </c>
       <c r="T123" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="U123" s="22" t="s">
         <v>233</v>
-      </c>
-      <c r="U123" s="22" t="s">
-        <v>232</v>
       </c>
       <c r="V123" s="22">
         <v>0</v>
@@ -9002,7 +9067,7 @@
     </row>
     <row r="124" s="6" customFormat="1" spans="1:22">
       <c r="A124" s="22" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B124" s="22">
         <v>1</v>
@@ -9018,7 +9083,7 @@
         <v>3</v>
       </c>
       <c r="G124" s="22" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H124" s="22"/>
       <c r="I124" s="22"/>
@@ -9047,10 +9112,10 @@
         <v>56</v>
       </c>
       <c r="T124" s="22" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="U124" s="22" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="V124" s="22">
         <v>0</v>
@@ -9058,7 +9123,7 @@
     </row>
     <row r="125" s="6" customFormat="1" spans="1:22">
       <c r="A125" s="22" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B125" s="22">
         <v>1</v>
@@ -9074,7 +9139,7 @@
         <v>4</v>
       </c>
       <c r="G125" s="22" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H125" s="22"/>
       <c r="I125" s="22"/>
@@ -9103,10 +9168,10 @@
         <v>56</v>
       </c>
       <c r="T125" s="22" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="U125" s="22" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="V125" s="22">
         <v>0</v>
@@ -9114,7 +9179,7 @@
     </row>
     <row r="126" s="6" customFormat="1" spans="1:22">
       <c r="A126" s="22" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B126" s="22">
         <v>1</v>
@@ -9130,7 +9195,7 @@
         <v>5</v>
       </c>
       <c r="G126" s="22" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H126" s="22"/>
       <c r="I126" s="22"/>
@@ -9159,10 +9224,10 @@
         <v>56</v>
       </c>
       <c r="T126" s="22" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="U126" s="22" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="V126" s="22">
         <v>0</v>
@@ -9170,7 +9235,7 @@
     </row>
     <row r="127" s="6" customFormat="1" spans="1:22">
       <c r="A127" s="22" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B127" s="22">
         <v>1</v>
@@ -9186,7 +9251,7 @@
         <v>6</v>
       </c>
       <c r="G127" s="22" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H127" s="22"/>
       <c r="I127" s="22"/>
@@ -9215,10 +9280,10 @@
         <v>56</v>
       </c>
       <c r="T127" s="22" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="U127" s="22" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="V127" s="22">
         <v>0</v>
@@ -9226,7 +9291,7 @@
     </row>
     <row r="128" s="6" customFormat="1" spans="1:22">
       <c r="A128" s="22" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B128" s="22">
         <v>1</v>
@@ -9242,7 +9307,7 @@
         <v>7</v>
       </c>
       <c r="G128" s="22" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H128" s="22"/>
       <c r="I128" s="22"/>
@@ -9271,10 +9336,10 @@
         <v>56</v>
       </c>
       <c r="T128" s="22" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="U128" s="22" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="V128" s="22">
         <v>0</v>
@@ -9282,7 +9347,7 @@
     </row>
     <row r="129" s="6" customFormat="1" spans="1:22">
       <c r="A129" s="22" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B129" s="22">
         <v>1</v>
@@ -9298,7 +9363,7 @@
         <v>8</v>
       </c>
       <c r="G129" s="22" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H129" s="22"/>
       <c r="I129" s="22"/>
@@ -9327,10 +9392,10 @@
         <v>56</v>
       </c>
       <c r="T129" s="22" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="U129" s="22" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="V129" s="22">
         <v>0</v>
@@ -9338,7 +9403,7 @@
     </row>
     <row r="130" s="6" customFormat="1" spans="1:22">
       <c r="A130" s="22" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B130" s="22">
         <v>1</v>
@@ -9354,7 +9419,7 @@
         <v>9</v>
       </c>
       <c r="G130" s="22" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H130" s="22"/>
       <c r="I130" s="22"/>
@@ -9383,10 +9448,10 @@
         <v>56</v>
       </c>
       <c r="T130" s="22" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="U130" s="22" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="V130" s="22">
         <v>0</v>
@@ -9394,7 +9459,7 @@
     </row>
     <row r="131" s="6" customFormat="1" spans="1:22">
       <c r="A131" s="22" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B131" s="22">
         <v>1</v>
@@ -9410,7 +9475,7 @@
         <v>10</v>
       </c>
       <c r="G131" s="22" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H131" s="22"/>
       <c r="I131" s="22"/>
@@ -9439,10 +9504,10 @@
         <v>56</v>
       </c>
       <c r="T131" s="22" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="U131" s="22" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="V131" s="22">
         <v>0</v>
@@ -9450,7 +9515,7 @@
     </row>
     <row r="132" s="8" customFormat="1" spans="1:22">
       <c r="A132" s="24" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B132" s="25">
         <v>3</v>
@@ -9466,7 +9531,7 @@
         <v>0</v>
       </c>
       <c r="G132" s="24" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="H132" s="25"/>
       <c r="I132" s="25"/>
@@ -9491,16 +9556,16 @@
       </c>
       <c r="Q132" s="25"/>
       <c r="R132" s="24" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="S132" s="12" t="s">
-        <v>56</v>
+        <v>246</v>
       </c>
       <c r="T132" s="24" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="U132" s="25" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="V132" s="25">
         <v>0</v>
@@ -9508,7 +9573,7 @@
     </row>
     <row r="133" s="8" customFormat="1" spans="1:22">
       <c r="A133" s="26" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B133" s="27">
         <v>3</v>
@@ -9524,7 +9589,7 @@
         <v>0</v>
       </c>
       <c r="G133" s="26" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="H133" s="27"/>
       <c r="I133" s="27"/>
@@ -9549,16 +9614,16 @@
       </c>
       <c r="Q133" s="27"/>
       <c r="R133" s="26" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="S133" s="12" t="s">
-        <v>56</v>
+        <v>246</v>
       </c>
       <c r="T133" s="26" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="U133" s="27" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="V133" s="27">
         <v>0</v>
@@ -9566,7 +9631,7 @@
     </row>
     <row r="134" s="8" customFormat="1" spans="1:22">
       <c r="A134" s="26" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B134" s="25">
         <v>3</v>
@@ -9582,7 +9647,7 @@
         <v>0</v>
       </c>
       <c r="G134" s="26" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="H134" s="27"/>
       <c r="I134" s="27"/>
@@ -9607,16 +9672,16 @@
       </c>
       <c r="Q134" s="27"/>
       <c r="R134" s="26" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="S134" s="12" t="s">
-        <v>56</v>
+        <v>246</v>
       </c>
       <c r="T134" s="26" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="U134" s="27" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="V134" s="27">
         <v>0</v>
@@ -9624,7 +9689,7 @@
     </row>
     <row r="135" s="8" customFormat="1" spans="1:22">
       <c r="A135" s="26" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="B135" s="27">
         <v>3</v>
@@ -9640,7 +9705,7 @@
         <v>0</v>
       </c>
       <c r="G135" s="26" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="H135" s="27"/>
       <c r="I135" s="27"/>
@@ -9665,16 +9730,16 @@
       </c>
       <c r="Q135" s="27"/>
       <c r="R135" s="26" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="S135" s="12" t="s">
-        <v>56</v>
+        <v>246</v>
       </c>
       <c r="T135" s="26" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="U135" s="27" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="V135" s="27">
         <v>0</v>
@@ -9682,7 +9747,7 @@
     </row>
     <row r="136" s="8" customFormat="1" spans="1:22">
       <c r="A136" s="26" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="B136" s="25">
         <v>3</v>
@@ -9698,7 +9763,7 @@
         <v>0</v>
       </c>
       <c r="G136" s="26" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="H136" s="27"/>
       <c r="I136" s="27"/>
@@ -9723,16 +9788,16 @@
       </c>
       <c r="Q136" s="27"/>
       <c r="R136" s="26" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="S136" s="12" t="s">
-        <v>56</v>
+        <v>246</v>
       </c>
       <c r="T136" s="26" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="U136" s="27" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="V136" s="27">
         <v>0</v>
@@ -9740,7 +9805,7 @@
     </row>
     <row r="137" s="8" customFormat="1" spans="1:22">
       <c r="A137" s="26" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="B137" s="27">
         <v>3</v>
@@ -9756,7 +9821,7 @@
         <v>0</v>
       </c>
       <c r="G137" s="26" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="H137" s="27"/>
       <c r="I137" s="27"/>
@@ -9781,25 +9846,199 @@
       </c>
       <c r="Q137" s="27"/>
       <c r="R137" s="26" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="S137" s="12" t="s">
-        <v>56</v>
+        <v>246</v>
       </c>
       <c r="T137" s="26" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="U137" s="27" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="V137" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" s="8" customFormat="1" spans="1:22">
+      <c r="A138" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="B138" s="27">
+        <v>3</v>
+      </c>
+      <c r="C138" s="27">
+        <v>1</v>
+      </c>
+      <c r="D138" s="27">
+        <v>1</v>
+      </c>
+      <c r="E138" s="27"/>
+      <c r="F138" s="27">
+        <v>0</v>
+      </c>
+      <c r="G138" s="26" t="s">
+        <v>275</v>
+      </c>
+      <c r="H138" s="27"/>
+      <c r="I138" s="27"/>
+      <c r="J138" s="29"/>
+      <c r="K138" s="27">
+        <v>0</v>
+      </c>
+      <c r="L138" s="27">
+        <v>0</v>
+      </c>
+      <c r="M138" s="27">
+        <v>1</v>
+      </c>
+      <c r="N138" s="27">
+        <v>0</v>
+      </c>
+      <c r="O138" s="25">
+        <v>1000</v>
+      </c>
+      <c r="P138" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q138" s="27"/>
+      <c r="R138" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="S138" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="T138" s="26" t="s">
+        <v>276</v>
+      </c>
+      <c r="U138" s="27" t="s">
+        <v>277</v>
+      </c>
+      <c r="V138" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" s="8" customFormat="1" spans="1:22">
+      <c r="A139" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="B139" s="27">
+        <v>3</v>
+      </c>
+      <c r="C139" s="27">
+        <v>1</v>
+      </c>
+      <c r="D139" s="27">
+        <v>1</v>
+      </c>
+      <c r="E139" s="27"/>
+      <c r="F139" s="27">
+        <v>0</v>
+      </c>
+      <c r="G139" s="26" t="s">
+        <v>279</v>
+      </c>
+      <c r="H139" s="27"/>
+      <c r="I139" s="27"/>
+      <c r="J139" s="29"/>
+      <c r="K139" s="27">
+        <v>0</v>
+      </c>
+      <c r="L139" s="27">
+        <v>0</v>
+      </c>
+      <c r="M139" s="27">
+        <v>1</v>
+      </c>
+      <c r="N139" s="27">
+        <v>0</v>
+      </c>
+      <c r="O139" s="25">
+        <v>1000</v>
+      </c>
+      <c r="P139" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q139" s="27"/>
+      <c r="R139" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="S139" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="T139" s="26" t="s">
+        <v>280</v>
+      </c>
+      <c r="U139" s="27" t="s">
+        <v>281</v>
+      </c>
+      <c r="V139" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" s="8" customFormat="1" spans="1:22">
+      <c r="A140" s="26" t="s">
+        <v>282</v>
+      </c>
+      <c r="B140" s="27">
+        <v>3</v>
+      </c>
+      <c r="C140" s="27">
+        <v>1</v>
+      </c>
+      <c r="D140" s="27">
+        <v>1</v>
+      </c>
+      <c r="E140" s="27"/>
+      <c r="F140" s="27">
+        <v>0</v>
+      </c>
+      <c r="G140" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="H140" s="27"/>
+      <c r="I140" s="27"/>
+      <c r="J140" s="29"/>
+      <c r="K140" s="27">
+        <v>0</v>
+      </c>
+      <c r="L140" s="27">
+        <v>0</v>
+      </c>
+      <c r="M140" s="27">
+        <v>1</v>
+      </c>
+      <c r="N140" s="27">
+        <v>0</v>
+      </c>
+      <c r="O140" s="25">
+        <v>1000</v>
+      </c>
+      <c r="P140" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q140" s="27"/>
+      <c r="R140" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="S140" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="T140" s="26" t="s">
+        <v>284</v>
+      </c>
+      <c r="U140" s="27" t="s">
+        <v>285</v>
+      </c>
+      <c r="V140" s="27">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A8"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S7:S8 B7:D8 T7:V8 E7:R8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:V8">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
remove unused define for item
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel_Ini/Item.xlsx
+++ b/_Out/NFDataCfg/Excel_Ini/Item.xlsx
@@ -890,9 +890,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22">
@@ -926,19 +926,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -957,9 +948,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -972,9 +977,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -988,36 +992,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -1026,10 +1000,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1050,14 +1025,39 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1102,31 +1102,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1138,7 +1144,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1150,7 +1156,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1162,31 +1198,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1198,55 +1210,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1264,19 +1228,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1359,7 +1359,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1367,8 +1367,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1404,21 +1404,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -1436,8 +1421,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1457,13 +1457,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1475,130 +1475,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2026,11 +2026,11 @@
   <dimension ref="A1:V140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="G40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B125" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J46" sqref="J46"/>
+      <selection pane="bottomRight" activeCell="D131" sqref="D131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -2851,7 +2851,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="14">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D13" s="14">
         <v>0</v>
@@ -2909,7 +2909,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="14">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D14" s="14">
         <v>0</v>
@@ -2967,7 +2967,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="14">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D15" s="14">
         <v>0</v>
@@ -3023,7 +3023,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="14">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D16" s="14">
         <v>0</v>
@@ -3079,7 +3079,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="14">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D17" s="14">
         <v>0</v>
@@ -3135,7 +3135,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="14">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D18" s="14">
         <v>0</v>
@@ -3191,7 +3191,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D19" s="14">
         <v>0</v>
@@ -3247,7 +3247,7 @@
         <v>2</v>
       </c>
       <c r="C20" s="14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D20" s="14">
         <v>0</v>
@@ -3303,7 +3303,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D21" s="14">
         <v>0</v>
@@ -3359,7 +3359,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D22" s="14">
         <v>0</v>
@@ -3415,7 +3415,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D23" s="14">
         <v>0</v>
@@ -3471,7 +3471,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D24" s="14">
         <v>0</v>
@@ -3527,7 +3527,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="14">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D25" s="14">
         <v>0</v>
@@ -3583,7 +3583,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="14">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D26" s="14">
         <v>0</v>
@@ -3639,7 +3639,7 @@
         <v>2</v>
       </c>
       <c r="C27" s="14">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D27" s="14">
         <v>0</v>
@@ -3695,7 +3695,7 @@
         <v>2</v>
       </c>
       <c r="C28" s="14">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D28" s="14">
         <v>0</v>
@@ -3751,7 +3751,7 @@
         <v>2</v>
       </c>
       <c r="C29" s="14">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D29" s="14">
         <v>0</v>
@@ -3807,7 +3807,7 @@
         <v>2</v>
       </c>
       <c r="C30" s="14">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D30" s="14">
         <v>0</v>
@@ -3863,7 +3863,7 @@
         <v>2</v>
       </c>
       <c r="C31" s="14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D31" s="14">
         <v>0</v>
@@ -3919,7 +3919,7 @@
         <v>2</v>
       </c>
       <c r="C32" s="14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D32" s="14">
         <v>0</v>
@@ -3975,7 +3975,7 @@
         <v>2</v>
       </c>
       <c r="C33" s="14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D33" s="14">
         <v>0</v>
@@ -4031,7 +4031,7 @@
         <v>2</v>
       </c>
       <c r="C34" s="14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D34" s="14">
         <v>0</v>
@@ -4087,7 +4087,7 @@
         <v>2</v>
       </c>
       <c r="C35" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D35" s="14">
         <v>0</v>
@@ -4143,7 +4143,7 @@
         <v>2</v>
       </c>
       <c r="C36" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D36" s="14">
         <v>0</v>
@@ -4199,7 +4199,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D37" s="14">
         <v>0</v>
@@ -4255,7 +4255,7 @@
         <v>2</v>
       </c>
       <c r="C38" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D38" s="14">
         <v>0</v>
@@ -4311,7 +4311,7 @@
         <v>2</v>
       </c>
       <c r="C39" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D39" s="14">
         <v>0</v>
@@ -4367,7 +4367,7 @@
         <v>2</v>
       </c>
       <c r="C40" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="14">
         <v>0</v>
@@ -4423,7 +4423,7 @@
         <v>2</v>
       </c>
       <c r="C41" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D41" s="14">
         <v>0</v>
@@ -4479,7 +4479,7 @@
         <v>2</v>
       </c>
       <c r="C42" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D42" s="14">
         <v>0</v>
@@ -4535,7 +4535,7 @@
         <v>2</v>
       </c>
       <c r="C43" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D43" s="14">
         <v>0</v>
@@ -4591,7 +4591,7 @@
         <v>2</v>
       </c>
       <c r="C44" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D44" s="14">
         <v>0</v>
@@ -4647,7 +4647,7 @@
         <v>2</v>
       </c>
       <c r="C45" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D45" s="14">
         <v>0</v>
@@ -4700,10 +4700,10 @@
         <v>138</v>
       </c>
       <c r="B46" s="17">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C46" s="17">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D46" s="17">
         <v>1</v>
@@ -4758,10 +4758,10 @@
         <v>142</v>
       </c>
       <c r="B47" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C47" s="17">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D47" s="17">
         <v>10</v>
@@ -4814,10 +4814,10 @@
         <v>143</v>
       </c>
       <c r="B48" s="17">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C48" s="17">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D48" s="17">
         <v>20</v>
@@ -4870,10 +4870,10 @@
         <v>144</v>
       </c>
       <c r="B49" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C49" s="17">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D49" s="17">
         <v>30</v>
@@ -4926,10 +4926,10 @@
         <v>145</v>
       </c>
       <c r="B50" s="17">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C50" s="17">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D50" s="17">
         <v>35</v>
@@ -4982,10 +4982,10 @@
         <v>146</v>
       </c>
       <c r="B51" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C51" s="17">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D51" s="17">
         <v>40</v>
@@ -5038,10 +5038,10 @@
         <v>147</v>
       </c>
       <c r="B52" s="17">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C52" s="17">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D52" s="17">
         <v>45</v>
@@ -5094,10 +5094,10 @@
         <v>148</v>
       </c>
       <c r="B53" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C53" s="17">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D53" s="17">
         <v>50</v>
@@ -5150,10 +5150,10 @@
         <v>149</v>
       </c>
       <c r="B54" s="17">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C54" s="17">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D54" s="17">
         <v>55</v>
@@ -5206,10 +5206,10 @@
         <v>150</v>
       </c>
       <c r="B55" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C55" s="17">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D55" s="17">
         <v>60</v>
@@ -5262,10 +5262,10 @@
         <v>151</v>
       </c>
       <c r="B56" s="17">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C56" s="17">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D56" s="17">
         <v>10</v>
@@ -5318,10 +5318,10 @@
         <v>154</v>
       </c>
       <c r="B57" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C57" s="17">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D57" s="17">
         <v>20</v>
@@ -5374,10 +5374,10 @@
         <v>155</v>
       </c>
       <c r="B58" s="17">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C58" s="17">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D58" s="17">
         <v>30</v>
@@ -5430,10 +5430,10 @@
         <v>156</v>
       </c>
       <c r="B59" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C59" s="17">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D59" s="17">
         <v>40</v>
@@ -5486,10 +5486,10 @@
         <v>157</v>
       </c>
       <c r="B60" s="17">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C60" s="17">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D60" s="20">
         <v>50</v>
@@ -5541,11 +5541,11 @@
       <c r="A61" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="B61" s="17">
-        <v>5</v>
+      <c r="B61" s="18">
+        <v>2</v>
       </c>
       <c r="C61" s="17">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D61" s="20">
         <v>60</v>
@@ -9521,7 +9521,7 @@
         <v>3</v>
       </c>
       <c r="C132" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D132" s="25">
         <v>1</v>
@@ -9579,7 +9579,7 @@
         <v>3</v>
       </c>
       <c r="C133" s="27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D133" s="27">
         <v>1</v>
@@ -9636,8 +9636,8 @@
       <c r="B134" s="25">
         <v>3</v>
       </c>
-      <c r="C134" s="27">
-        <v>1</v>
+      <c r="C134" s="25">
+        <v>0</v>
       </c>
       <c r="D134" s="27">
         <v>1</v>
@@ -9695,7 +9695,7 @@
         <v>3</v>
       </c>
       <c r="C135" s="27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D135" s="27">
         <v>1</v>
@@ -9752,8 +9752,8 @@
       <c r="B136" s="25">
         <v>3</v>
       </c>
-      <c r="C136" s="27">
-        <v>1</v>
+      <c r="C136" s="25">
+        <v>0</v>
       </c>
       <c r="D136" s="27">
         <v>1</v>
@@ -9811,7 +9811,7 @@
         <v>3</v>
       </c>
       <c r="C137" s="27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D137" s="27">
         <v>1</v>
@@ -9868,8 +9868,8 @@
       <c r="B138" s="27">
         <v>3</v>
       </c>
-      <c r="C138" s="27">
-        <v>1</v>
+      <c r="C138" s="25">
+        <v>0</v>
       </c>
       <c r="D138" s="27">
         <v>1</v>
@@ -9927,7 +9927,7 @@
         <v>3</v>
       </c>
       <c r="C139" s="27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D139" s="27">
         <v>1</v>
@@ -9984,8 +9984,8 @@
       <c r="B140" s="27">
         <v>3</v>
       </c>
-      <c r="C140" s="27">
-        <v>1</v>
+      <c r="C140" s="25">
+        <v>0</v>
       </c>
       <c r="D140" s="27">
         <v>1</v>

</xml_diff>

<commit_message>
add sprites fixed bug for switch hero
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel_Ini/Item.xlsx
+++ b/_Out/NFDataCfg/Excel_Ini/Item.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="478">
   <si>
     <t>Id</t>
   </si>
@@ -1461,6 +1461,9 @@
   </si>
   <si>
     <t>Build_mana_well_3</t>
+  </si>
+  <si>
+    <t>UIResources/BuilderSprite</t>
   </si>
 </sst>
 </file>
@@ -2074,10 +2077,10 @@
   <dimension ref="A1:V176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="O166" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="O164" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="R141" sqref="R141:R176"/>
+      <selection pane="bottomRight" activeCell="S141" sqref="S141:S176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -10128,7 +10131,7 @@
         <v>441</v>
       </c>
       <c r="S141" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T141" s="32" t="s">
         <v>405</v>
@@ -10186,7 +10189,7 @@
         <v>442</v>
       </c>
       <c r="S142" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T142" s="32" t="s">
         <v>406</v>
@@ -10244,7 +10247,7 @@
         <v>443</v>
       </c>
       <c r="S143" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T143" s="32" t="s">
         <v>407</v>
@@ -10302,7 +10305,7 @@
         <v>444</v>
       </c>
       <c r="S144" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T144" s="32" t="s">
         <v>408</v>
@@ -10360,7 +10363,7 @@
         <v>445</v>
       </c>
       <c r="S145" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T145" s="32" t="s">
         <v>409</v>
@@ -10418,7 +10421,7 @@
         <v>446</v>
       </c>
       <c r="S146" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T146" s="32" t="s">
         <v>410</v>
@@ -10476,7 +10479,7 @@
         <v>447</v>
       </c>
       <c r="S147" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T147" s="32" t="s">
         <v>411</v>
@@ -10534,7 +10537,7 @@
         <v>448</v>
       </c>
       <c r="S148" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T148" s="32" t="s">
         <v>412</v>
@@ -10592,7 +10595,7 @@
         <v>449</v>
       </c>
       <c r="S149" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T149" s="32" t="s">
         <v>413</v>
@@ -10650,7 +10653,7 @@
         <v>450</v>
       </c>
       <c r="S150" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T150" s="32" t="s">
         <v>414</v>
@@ -10708,7 +10711,7 @@
         <v>451</v>
       </c>
       <c r="S151" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T151" s="32" t="s">
         <v>415</v>
@@ -10766,7 +10769,7 @@
         <v>452</v>
       </c>
       <c r="S152" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T152" s="32" t="s">
         <v>416</v>
@@ -10824,7 +10827,7 @@
         <v>453</v>
       </c>
       <c r="S153" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T153" s="32" t="s">
         <v>417</v>
@@ -10882,7 +10885,7 @@
         <v>454</v>
       </c>
       <c r="S154" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T154" s="32" t="s">
         <v>418</v>
@@ -10940,7 +10943,7 @@
         <v>455</v>
       </c>
       <c r="S155" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T155" s="32" t="s">
         <v>419</v>
@@ -10998,7 +11001,7 @@
         <v>456</v>
       </c>
       <c r="S156" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T156" s="32" t="s">
         <v>420</v>
@@ -11056,7 +11059,7 @@
         <v>457</v>
       </c>
       <c r="S157" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T157" s="32" t="s">
         <v>421</v>
@@ -11114,7 +11117,7 @@
         <v>458</v>
       </c>
       <c r="S158" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T158" s="32" t="s">
         <v>422</v>
@@ -11172,7 +11175,7 @@
         <v>459</v>
       </c>
       <c r="S159" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T159" s="32" t="s">
         <v>423</v>
@@ -11230,7 +11233,7 @@
         <v>460</v>
       </c>
       <c r="S160" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T160" s="32" t="s">
         <v>424</v>
@@ -11288,7 +11291,7 @@
         <v>461</v>
       </c>
       <c r="S161" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T161" s="32" t="s">
         <v>425</v>
@@ -11346,7 +11349,7 @@
         <v>462</v>
       </c>
       <c r="S162" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T162" s="32" t="s">
         <v>426</v>
@@ -11404,7 +11407,7 @@
         <v>463</v>
       </c>
       <c r="S163" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T163" s="32" t="s">
         <v>427</v>
@@ -11462,7 +11465,7 @@
         <v>464</v>
       </c>
       <c r="S164" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T164" s="32" t="s">
         <v>428</v>
@@ -11520,7 +11523,7 @@
         <v>465</v>
       </c>
       <c r="S165" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T165" s="32" t="s">
         <v>429</v>
@@ -11578,7 +11581,7 @@
         <v>466</v>
       </c>
       <c r="S166" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T166" s="32" t="s">
         <v>430</v>
@@ -11636,7 +11639,7 @@
         <v>467</v>
       </c>
       <c r="S167" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T167" s="32" t="s">
         <v>431</v>
@@ -11694,7 +11697,7 @@
         <v>468</v>
       </c>
       <c r="S168" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T168" s="32" t="s">
         <v>432</v>
@@ -11752,7 +11755,7 @@
         <v>469</v>
       </c>
       <c r="S169" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T169" s="32" t="s">
         <v>433</v>
@@ -11810,7 +11813,7 @@
         <v>470</v>
       </c>
       <c r="S170" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T170" s="32" t="s">
         <v>434</v>
@@ -11868,7 +11871,7 @@
         <v>471</v>
       </c>
       <c r="S171" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T171" s="32" t="s">
         <v>435</v>
@@ -11926,7 +11929,7 @@
         <v>472</v>
       </c>
       <c r="S172" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T172" s="32" t="s">
         <v>436</v>
@@ -11984,7 +11987,7 @@
         <v>473</v>
       </c>
       <c r="S173" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T173" s="32" t="s">
         <v>437</v>
@@ -12042,7 +12045,7 @@
         <v>474</v>
       </c>
       <c r="S174" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T174" s="32" t="s">
         <v>438</v>
@@ -12100,7 +12103,7 @@
         <v>475</v>
       </c>
       <c r="S175" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T175" s="32" t="s">
         <v>439</v>
@@ -12158,7 +12161,7 @@
         <v>476</v>
       </c>
       <c r="S176" s="33" t="s">
-        <v>282</v>
+        <v>477</v>
       </c>
       <c r="T176" s="32" t="s">
         <v>440</v>

</xml_diff>